<commit_message>
fix: ob import open to all
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-officialbus-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-officialbus-template.xlsx
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lambert\accupay\AccuPay\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kzi4GFhAB0fOYKThsR2OQBd5fcZGZTJMlGx9aHppdbYHdT9TbF129UwTSxMUFHnaW2pcCn6eI4XmT/xT2YTeKw==" workbookSaltValue="WGOu0//xxe7J9eCkEBmHfQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -45,13 +46,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,11 +82,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,39 +372,42 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="1023" max="1025" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="1022" width="8.7109375" style="3"/>
+    <col min="1023" max="1025" width="11.5703125" style="3" customWidth="1"/>
+    <col min="1026" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9BGFevB+LRkN9OrdgZ5cjsekoK5WYVX6P3eflYPwc6QB/QoN5g2Qtc5vPycup6WGjiMYBrjs0TPYTTBTU6AqJg==" saltValue="UU0PMz5tYp70z8DoXxO6ig==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Peqv5pmKarb6spKN++DrKoVGMdhDmzVlXqqxXZXSifB7v68LU4s8GlDtG7CHwLlGgXP73KWTRa5qe1zHxHyArg==" saltValue="LzZGknDGwzhIuhwz/9OYuw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>